<commit_message>
Edit: etc 파일 변경:
</commit_message>
<xml_diff>
--- a/etc/collaborator_list.xlsx
+++ b/etc/collaborator_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DLAB_Y\Desktop\JIONI\Homepages\dlab-amc.github.io\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD895879-B0D5-4CD4-A984-02BB74C7ED2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B001D1-2F66-44F2-AC97-877468CD7424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14880" yWindow="-2100" windowWidth="12150" windowHeight="20745" xr2:uid="{8DD8C801-A878-431B-B905-38027FC838F7}"/>
+    <workbookView xWindow="-14415" yWindow="1110" windowWidth="12150" windowHeight="20745" xr2:uid="{8DD8C801-A878-431B-B905-38027FC838F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>인제대학교 해운대백병원 진단검사의학과</t>
   </si>
   <si>
-    <t>부산대학교병원  진단검사의학과</t>
-  </si>
-  <si>
     <t>울산대학교 서울아산병원 정형외과</t>
   </si>
   <si>
@@ -146,6 +143,10 @@
   </si>
   <si>
     <t>영문 병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산대학교병원 진단검사의학과</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -533,7 +534,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -545,58 +546,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -604,26 +605,26 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -631,25 +632,25 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -660,5 +661,6 @@
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>